<commit_message>
Code Version 2018/4/6, Ettrore_icf_sc 1.2HF update - psudo-BCS
</commit_message>
<xml_diff>
--- a/Fortran code/Fortran_gdqmc_icf_pin/Record/Record.xlsx
+++ b/Fortran code/Fortran_gdqmc_icf_pin/Record/Record.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783E36C0-C8A1-453F-BBD0-505F8171F324}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="157">
   <si>
     <t>Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -539,6 +540,93 @@
   </si>
   <si>
     <t>/sciclone/pscr/zxiao01/run/gdqmc_icf_pin2.0_d_muti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/26/2018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2DET u4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculated but don’t know why not saved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2DET_u4</t>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2DET u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2DET u12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2DET_u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2DET_u12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2x_u4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2x_u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2x_u12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2x u4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2x u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2x u12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2xx u4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2xx u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpqmc_bcs1.2xx u12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2xx_u4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2xx_u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sciclone/pscr/zxiao01/run/cpqmc_bcs1.2xx_u12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -890,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+    <sheetView tabSelected="1" topLeftCell="D100" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1731,7 +1819,9 @@
       <c r="C76" t="s">
         <v>77</v>
       </c>
-      <c r="D76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="E76" t="s">
         <v>118</v>
       </c>
@@ -1990,7 +2080,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>133</v>
       </c>
@@ -1999,20 +2089,167 @@
       </c>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C114" t="s">
         <v>9</v>
       </c>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>135</v>
+      </c>
+      <c r="B118" t="s">
+        <v>136</v>
+      </c>
+      <c r="C118" t="s">
+        <v>137</v>
+      </c>
+      <c r="E118" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E119" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
+        <v>141</v>
+      </c>
+      <c r="C120" t="s">
+        <v>137</v>
+      </c>
+      <c r="E120" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E121" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>142</v>
+      </c>
+      <c r="C122" t="s">
+        <v>137</v>
+      </c>
+      <c r="E122" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E123" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
+        <v>148</v>
+      </c>
+      <c r="C124" t="s">
+        <v>137</v>
+      </c>
+      <c r="E124" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E125" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B126" t="s">
+        <v>149</v>
+      </c>
+      <c r="C126" t="s">
+        <v>137</v>
+      </c>
+      <c r="E126" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E127" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>150</v>
+      </c>
+      <c r="C128" t="s">
+        <v>137</v>
+      </c>
+      <c r="E128" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E129" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
+        <v>151</v>
+      </c>
+      <c r="C130" t="s">
+        <v>137</v>
+      </c>
+      <c r="E130" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E131" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B132" t="s">
+        <v>152</v>
+      </c>
+      <c r="C132" t="s">
+        <v>137</v>
+      </c>
+      <c r="E132" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E133" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>153</v>
+      </c>
+      <c r="C134" t="s">
+        <v>137</v>
+      </c>
+      <c r="E134" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E135" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>